<commit_message>
Update docs for week 1
</commit_message>
<xml_diff>
--- a/docs/Group-2-Sprint_Planning_Document.xlsx
+++ b/docs/Group-2-Sprint_Planning_Document.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyled\Desktop\ctu\CS-Group-Project-2\Group-2-Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6C32A0-3860-4494-B034-2B497C4A942E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5958913E-7801-4FDD-BD87-4E5B8C8A07BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="30" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="142">
   <si>
     <t>What is this?</t>
   </si>
@@ -511,6 +511,12 @@
   </si>
   <si>
     <t>Logged-in customers can leave star ratings and written reviews for books they purchased.</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Week 1 Progress</t>
   </si>
 </sst>
 </file>
@@ -680,7 +686,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -711,6 +717,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -1109,7 +1121,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1426,6 +1438,26 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2602,16 +2634,16 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>#N/A</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>#N/A</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>#N/A</c:v>
@@ -3458,7 +3490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511F918D-DD7E-4456-AFA8-D34E9B85BCAC}">
   <dimension ref="A2:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -4582,8 +4614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91ABC362-0AA8-49DD-9635-2911E550F792}">
   <dimension ref="A2:S54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5158,21 +5190,37 @@
       <c r="S22" s="18"/>
     </row>
     <row r="23" spans="1:19" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="65"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="66"/>
+      <c r="B23" s="100" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="101" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="102" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="103">
+        <v>8</v>
+      </c>
       <c r="F23" s="50"/>
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="50"/>
+      <c r="J23" s="18">
+        <v>2</v>
+      </c>
+      <c r="K23" s="18">
+        <v>1</v>
+      </c>
+      <c r="L23" s="18">
+        <v>3</v>
+      </c>
+      <c r="M23" s="50">
+        <v>2</v>
+      </c>
       <c r="N23" s="18"/>
       <c r="O23" s="18"/>
       <c r="P23" s="18"/>
@@ -5341,21 +5389,21 @@
         <f>IF(SUM(I12:I27)&gt;0,E29-SUM(F12:I27),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="J30" s="7" t="e">
+      <c r="J30" s="7">
         <f>IF(SUM(J12:J27)&gt;0,E29-SUM(F12:J27),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K30" s="7" t="e">
+        <v>62</v>
+      </c>
+      <c r="K30" s="7">
         <f>IF(SUM(K12:K27)&gt;0,E29-SUM(F12:K27),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L30" s="7" t="e">
+        <v>61</v>
+      </c>
+      <c r="L30" s="7">
         <f>IF(SUM(L12:L27)&gt;0,E29-SUM(F12:L27),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M30" s="7" t="e">
+        <v>58</v>
+      </c>
+      <c r="M30" s="7">
         <f>IF(SUM(M12:M27)&gt;0,L30-SUM(M12:M27),NA())</f>
-        <v>#N/A</v>
+        <v>56</v>
       </c>
       <c r="N30" s="7" t="e">
         <f>IF(SUM(N12:N27)&gt;0,L30-SUM(M12:N27),NA())</f>
@@ -5482,7 +5530,7 @@
       </c>
       <c r="L36" s="3">
         <f>SUM(E12:E28)</f>
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
@@ -5494,7 +5542,7 @@
       </c>
       <c r="S36" s="3">
         <f>SUM(L12:L29)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="11:19" x14ac:dyDescent="0.2">
@@ -5706,8 +5754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08C063E-F911-44D8-941E-DFF238D0F4B4}">
   <dimension ref="A2:EC32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update repo for Week 2 contributions
</commit_message>
<xml_diff>
--- a/docs/Group-2-Sprint_Planning_Document.xlsx
+++ b/docs/Group-2-Sprint_Planning_Document.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyled\Desktop\ctu\CS-Group-Project-2\Group-2-Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D9D635-CDA3-45B3-B450-68B4F2315593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C53C214-8758-4232-8ED6-EE1215AC9A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19035" yWindow="3375" windowWidth="25545" windowHeight="15465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="30" r:id="rId1"/>
@@ -1388,45 +1388,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1461,6 +1422,45 @@
     <xf numFmtId="0" fontId="21" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1468,6 +1468,32 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <font>
+        <i val="0"/>
+        <sz val="12"/>
+        <name val="Times New Roman"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="41"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1490,7 +1516,7 @@
           <bgColor indexed="41"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1560,35 +1586,7 @@
           <bgColor indexed="41"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-        <sz val="12"/>
-        <name val="Times New Roman"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="41"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1629,7 +1627,9 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -2634,19 +2634,19 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>62</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>58</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>56</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>#N/A</c:v>
@@ -3218,11 +3218,11 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CAB15286-4F1A-419E-9263-9C0A08B60A81}" name=" Story ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{B74C3C53-A2BB-4E45-9F15-8AD5EB55830C}" name="Title" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{20E09014-6B26-4A59-8D85-43BDCB031975}" name="Description" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{04035D57-5E48-45CC-8A17-A398C0AF4A44}" name="Acceptance Criteria" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{0BBB23D4-203B-46EF-91A6-B64A342742C8}" name="Priority #" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{5E12523F-7857-4BD9-98C6-370258EF5CB5}" name="Sprint #" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{BEB5CABA-6DB7-4381-8096-9EBEC99BBF50}" name="Responsibility" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{20E09014-6B26-4A59-8D85-43BDCB031975}" name="Description" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{04035D57-5E48-45CC-8A17-A398C0AF4A44}" name="Acceptance Criteria" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{0BBB23D4-203B-46EF-91A6-B64A342742C8}" name="Priority #" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{5E12523F-7857-4BD9-98C6-370258EF5CB5}" name="Sprint #" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{BEB5CABA-6DB7-4381-8096-9EBEC99BBF50}" name="Responsibility" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3522,21 +3522,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="str">
+      <c r="A2" s="91" t="str">
         <f>CONCATENATE("Sprint #1",E5, "Tracking Sheet")</f>
         <v>Sprint #1Tracking Sheet</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
     </row>
     <row r="4" spans="1:19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -3544,15 +3544,15 @@
       <c r="C4" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="84"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="94"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C5" s="47" t="s">
@@ -3591,24 +3591,24 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="85" t="s">
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="N9" s="86"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="86"/>
-      <c r="R9" s="86"/>
-      <c r="S9" s="87"/>
+      <c r="N9" s="96"/>
+      <c r="O9" s="96"/>
+      <c r="P9" s="96"/>
+      <c r="Q9" s="96"/>
+      <c r="R9" s="96"/>
+      <c r="S9" s="97"/>
     </row>
     <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F10" s="40">
@@ -3762,10 +3762,10 @@
       <c r="A13" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="97" t="s">
+      <c r="B13" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="82" t="s">
         <v>100</v>
       </c>
       <c r="D13" s="60" t="s">
@@ -3793,10 +3793,10 @@
       <c r="A14" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="82" t="s">
         <v>101</v>
       </c>
       <c r="D14" s="60" t="s">
@@ -3824,10 +3824,10 @@
       <c r="A15" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="97" t="s">
+      <c r="B15" s="84" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="82" t="s">
         <v>104</v>
       </c>
       <c r="D15" s="60" t="s">
@@ -3855,10 +3855,10 @@
       <c r="A16" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="97" t="s">
+      <c r="B16" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="95" t="s">
+      <c r="C16" s="82" t="s">
         <v>106</v>
       </c>
       <c r="D16" s="60" t="s">
@@ -3886,10 +3886,10 @@
       <c r="A17" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="97" t="s">
+      <c r="B17" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="95" t="s">
+      <c r="C17" s="82" t="s">
         <v>108</v>
       </c>
       <c r="D17" s="60" t="s">
@@ -3917,10 +3917,10 @@
       <c r="A18" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="95" t="s">
+      <c r="C18" s="82" t="s">
         <v>110</v>
       </c>
       <c r="D18" s="60" t="s">
@@ -3948,10 +3948,10 @@
       <c r="A19" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="97" t="s">
+      <c r="B19" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="82" t="s">
         <v>96</v>
       </c>
       <c r="D19" s="63" t="s">
@@ -3979,10 +3979,10 @@
       <c r="A20" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="95" t="s">
+      <c r="C20" s="82" t="s">
         <v>113</v>
       </c>
       <c r="D20" s="63" t="s">
@@ -4010,10 +4010,10 @@
       <c r="A21" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="97" t="s">
+      <c r="B21" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="95" t="s">
+      <c r="C21" s="82" t="s">
         <v>115</v>
       </c>
       <c r="D21" s="63" t="s">
@@ -4041,10 +4041,10 @@
       <c r="A22" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="97" t="s">
+      <c r="B22" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="95" t="s">
+      <c r="C22" s="82" t="s">
         <v>117</v>
       </c>
       <c r="D22" s="63" t="s">
@@ -4211,7 +4211,7 @@
         <v>24</v>
       </c>
       <c r="D29" s="38"/>
-      <c r="E29" s="88">
+      <c r="E29" s="98">
         <f>8*2*E8</f>
         <v>64</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>25</v>
       </c>
       <c r="D30" s="39"/>
-      <c r="E30" s="89"/>
+      <c r="E30" s="99"/>
       <c r="F30" s="7" t="e">
         <f>IF(SUM(F12:F27)&gt;0,E29-SUM(F12:F27),NA())</f>
         <v>#N/A</v>
@@ -4617,8 +4617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91ABC362-0AA8-49DD-9635-2911E550F792}">
   <dimension ref="A2:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4646,21 +4646,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="str">
+      <c r="A2" s="91" t="str">
         <f>CONCATENATE("Sprint #1",E5, "Tracking Sheet")</f>
         <v>Sprint #1Tracking Sheet</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
     </row>
     <row r="4" spans="1:19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -4668,15 +4668,15 @@
       <c r="C4" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="84"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="94"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C5" s="47" t="s">
@@ -4715,24 +4715,24 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="85" t="s">
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="N9" s="86"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="86"/>
-      <c r="R9" s="86"/>
-      <c r="S9" s="87"/>
+      <c r="N9" s="96"/>
+      <c r="O9" s="96"/>
+      <c r="P9" s="96"/>
+      <c r="Q9" s="96"/>
+      <c r="R9" s="96"/>
+      <c r="S9" s="97"/>
     </row>
     <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F10" s="40">
@@ -4886,7 +4886,7 @@
       <c r="A13" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="83" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="77" t="s">
@@ -4900,11 +4900,17 @@
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
+      <c r="H13" s="22">
+        <v>2</v>
+      </c>
+      <c r="I13" s="22">
+        <v>2</v>
+      </c>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
+      <c r="L13" s="21">
+        <v>2</v>
+      </c>
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
       <c r="O13" s="22"/>
@@ -4917,7 +4923,7 @@
       <c r="A14" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="96" t="s">
+      <c r="B14" s="83" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="77" t="s">
@@ -4932,7 +4938,9 @@
       <c r="F14" s="22"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
+      <c r="I14" s="21">
+        <v>2</v>
+      </c>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
@@ -4948,7 +4956,7 @@
       <c r="A15" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="83" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="77" t="s">
@@ -4964,7 +4972,9 @@
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="J15" s="21">
+        <v>1</v>
+      </c>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="22"/>
@@ -4979,7 +4989,7 @@
       <c r="A16" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="83" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="77" t="s">
@@ -4996,7 +5006,9 @@
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="K16" s="21">
+        <v>2</v>
+      </c>
       <c r="L16" s="21"/>
       <c r="M16" s="22"/>
       <c r="N16" s="21"/>
@@ -5010,7 +5022,7 @@
       <c r="A17" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="83" t="s">
         <v>62</v>
       </c>
       <c r="C17" s="77" t="s">
@@ -5028,7 +5040,9 @@
       <c r="I17" s="21"/>
       <c r="J17" s="21"/>
       <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
+      <c r="L17" s="21">
+        <v>2</v>
+      </c>
       <c r="M17" s="22"/>
       <c r="N17" s="21"/>
       <c r="O17" s="21"/>
@@ -5041,7 +5055,7 @@
       <c r="A18" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="83" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="77" t="s">
@@ -5072,7 +5086,7 @@
       <c r="A19" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="83" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="77" t="s">
@@ -5089,7 +5103,9 @@
       <c r="H19" s="51"/>
       <c r="I19" s="51"/>
       <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
+      <c r="K19" s="51">
+        <v>2</v>
+      </c>
       <c r="L19" s="51"/>
       <c r="M19" s="22"/>
       <c r="N19" s="51"/>
@@ -5103,7 +5119,7 @@
       <c r="A20" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="96" t="s">
+      <c r="B20" s="83" t="s">
         <v>42</v>
       </c>
       <c r="C20" s="77" t="s">
@@ -5117,9 +5133,13 @@
       </c>
       <c r="F20" s="22"/>
       <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
+      <c r="H20" s="18">
+        <v>3</v>
+      </c>
       <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="J20" s="18">
+        <v>1</v>
+      </c>
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
       <c r="M20" s="22"/>
@@ -5134,7 +5154,7 @@
       <c r="A21" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="96" t="s">
+      <c r="B21" s="83" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="77" t="s">
@@ -5149,7 +5169,9 @@
       <c r="F21" s="50"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="I21" s="18">
+        <v>0</v>
+      </c>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="18"/>
@@ -5165,7 +5187,7 @@
       <c r="A22" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="83" t="s">
         <v>44</v>
       </c>
       <c r="C22" s="77" t="s">
@@ -5180,7 +5202,9 @@
       <c r="F22" s="50"/>
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
+      <c r="I22" s="18">
+        <v>0</v>
+      </c>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
@@ -5193,19 +5217,19 @@
       <c r="S22" s="18"/>
     </row>
     <row r="23" spans="1:19" s="73" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="99" t="s">
+      <c r="A23" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="100" t="s">
+      <c r="B23" s="87" t="s">
         <v>141</v>
       </c>
-      <c r="C23" s="101" t="s">
+      <c r="C23" s="88" t="s">
         <v>142</v>
       </c>
-      <c r="D23" s="102" t="s">
+      <c r="D23" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="103">
+      <c r="E23" s="90">
         <v>8</v>
       </c>
       <c r="F23" s="50"/>
@@ -5351,7 +5375,7 @@
         <v>24</v>
       </c>
       <c r="D29" s="38"/>
-      <c r="E29" s="88">
+      <c r="E29" s="98">
         <f>8*2*E8</f>
         <v>64</v>
       </c>
@@ -5375,7 +5399,7 @@
         <v>25</v>
       </c>
       <c r="D30" s="39"/>
-      <c r="E30" s="89"/>
+      <c r="E30" s="99"/>
       <c r="F30" s="7" t="e">
         <f>IF(SUM(F12:F27)&gt;0,E29-SUM(F12:F27),NA())</f>
         <v>#N/A</v>
@@ -5388,25 +5412,25 @@
         <f>IF(SUM(H12:H27)&gt;0,F30-SUM(G12:H27),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="I30" s="7" t="e">
+      <c r="I30" s="7">
         <f>IF(SUM(I12:I27)&gt;0,E29-SUM(F12:I27),NA())</f>
-        <v>#N/A</v>
+        <v>55</v>
       </c>
       <c r="J30" s="7">
         <f>IF(SUM(J12:J27)&gt;0,E29-SUM(F12:J27),NA())</f>
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="K30" s="7">
         <f>IF(SUM(K12:K27)&gt;0,E29-SUM(F12:K27),NA())</f>
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="L30" s="7">
         <f>IF(SUM(L12:L27)&gt;0,E29-SUM(F12:L27),NA())</f>
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="M30" s="7">
         <f>IF(SUM(M12:M27)&gt;0,L30-SUM(M12:M27),NA())</f>
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="N30" s="7" t="e">
         <f>IF(SUM(N12:N27)&gt;0,L30-SUM(M12:N27),NA())</f>
@@ -5545,7 +5569,7 @@
       </c>
       <c r="S36" s="3">
         <f>SUM(L12:L29)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="11:19" x14ac:dyDescent="0.2">
@@ -5775,14 +5799,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:133" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
     </row>
     <row r="3" spans="1:133" x14ac:dyDescent="0.25">
       <c r="D3" s="34"/>
@@ -7455,25 +7479,25 @@
       <c r="EC20" s="45"/>
     </row>
     <row r="21" spans="1:133" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="94" t="s">
+      <c r="A21" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="94" t="s">
+      <c r="C21" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="98" t="s">
+      <c r="D21" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="E21" s="94">
+      <c r="E21" s="81">
         <v>2</v>
       </c>
-      <c r="F21" s="94">
+      <c r="F21" s="81">
         <v>2</v>
       </c>
-      <c r="G21" s="94"/>
+      <c r="G21" s="81"/>
       <c r="H21" s="45"/>
       <c r="I21" s="45"/>
       <c r="J21" s="45"/>
@@ -7602,46 +7626,46 @@
       <c r="EC21" s="45"/>
     </row>
     <row r="22" spans="1:133" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="94" t="s">
+      <c r="B22" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="94" t="s">
+      <c r="C22" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="D22" s="98" t="s">
+      <c r="D22" s="85" t="s">
         <v>132</v>
       </c>
-      <c r="E22" s="94">
+      <c r="E22" s="81">
         <v>2</v>
       </c>
-      <c r="F22" s="94">
+      <c r="F22" s="81">
         <v>2</v>
       </c>
-      <c r="G22" s="94"/>
+      <c r="G22" s="81"/>
     </row>
     <row r="23" spans="1:133" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="94" t="s">
+      <c r="B23" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="94" t="s">
+      <c r="C23" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="98" t="s">
+      <c r="D23" s="85" t="s">
         <v>133</v>
       </c>
-      <c r="E23" s="94">
+      <c r="E23" s="81">
         <v>2</v>
       </c>
-      <c r="F23" s="94">
+      <c r="F23" s="81">
         <v>2</v>
       </c>
-      <c r="G23" s="94"/>
+      <c r="G23" s="81"/>
       <c r="DW23" s="33"/>
       <c r="DX23" s="33"/>
       <c r="DY23" s="33"/>
@@ -7651,25 +7675,25 @@
       <c r="EC23" s="33"/>
     </row>
     <row r="24" spans="1:133" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="94" t="s">
+      <c r="B24" s="81" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="94" t="s">
+      <c r="C24" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="98" t="s">
+      <c r="D24" s="85" t="s">
         <v>134</v>
       </c>
-      <c r="E24" s="94">
+      <c r="E24" s="81">
         <v>2</v>
       </c>
-      <c r="F24" s="94">
+      <c r="F24" s="81">
         <v>2</v>
       </c>
-      <c r="G24" s="94"/>
+      <c r="G24" s="81"/>
       <c r="DW24" s="33"/>
       <c r="DX24" s="33"/>
       <c r="DY24" s="33"/>
@@ -7679,25 +7703,25 @@
       <c r="EC24" s="33"/>
     </row>
     <row r="25" spans="1:133" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="94" t="s">
+      <c r="B25" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="94" t="s">
+      <c r="C25" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="98" t="s">
+      <c r="D25" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="E25" s="94">
+      <c r="E25" s="81">
         <v>2</v>
       </c>
-      <c r="F25" s="94">
+      <c r="F25" s="81">
         <v>2</v>
       </c>
-      <c r="G25" s="94"/>
+      <c r="G25" s="81"/>
       <c r="DW25" s="33"/>
       <c r="DX25" s="33"/>
       <c r="DY25" s="33"/>
@@ -7707,25 +7731,25 @@
       <c r="EC25" s="33"/>
     </row>
     <row r="26" spans="1:133" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="94" t="s">
+      <c r="A26" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="94" t="s">
+      <c r="C26" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="98" t="s">
+      <c r="D26" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="E26" s="94">
+      <c r="E26" s="81">
         <v>2</v>
       </c>
-      <c r="F26" s="94">
+      <c r="F26" s="81">
         <v>2</v>
       </c>
-      <c r="G26" s="94"/>
+      <c r="G26" s="81"/>
       <c r="DW26" s="33"/>
       <c r="DX26" s="33"/>
       <c r="DY26" s="33"/>
@@ -7735,25 +7759,25 @@
       <c r="EC26" s="33"/>
     </row>
     <row r="27" spans="1:133" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="94" t="s">
+      <c r="A27" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="94" t="s">
+      <c r="C27" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="98" t="s">
+      <c r="D27" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="E27" s="94">
+      <c r="E27" s="81">
         <v>2</v>
       </c>
-      <c r="F27" s="94">
+      <c r="F27" s="81">
         <v>2</v>
       </c>
-      <c r="G27" s="94"/>
+      <c r="G27" s="81"/>
       <c r="DW27" s="33"/>
       <c r="DX27" s="33"/>
       <c r="DY27" s="33"/>
@@ -7763,25 +7787,25 @@
       <c r="EC27" s="33"/>
     </row>
     <row r="28" spans="1:133" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="94" t="s">
+      <c r="A28" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="94" t="s">
+      <c r="B28" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="94" t="s">
+      <c r="C28" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="98" t="s">
+      <c r="D28" s="85" t="s">
         <v>138</v>
       </c>
-      <c r="E28" s="94">
+      <c r="E28" s="81">
         <v>2</v>
       </c>
-      <c r="F28" s="94">
+      <c r="F28" s="81">
         <v>2</v>
       </c>
-      <c r="G28" s="94"/>
+      <c r="G28" s="81"/>
       <c r="DW28" s="33"/>
       <c r="DX28" s="33"/>
       <c r="DY28" s="33"/>
@@ -7791,25 +7815,25 @@
       <c r="EC28" s="33"/>
     </row>
     <row r="29" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A29" s="94" t="s">
+      <c r="A29" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="94" t="s">
+      <c r="B29" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="94" t="s">
+      <c r="C29" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="D29" s="98" t="s">
+      <c r="D29" s="85" t="s">
         <v>139</v>
       </c>
-      <c r="E29" s="94">
+      <c r="E29" s="81">
         <v>2</v>
       </c>
-      <c r="F29" s="94">
+      <c r="F29" s="81">
         <v>2</v>
       </c>
-      <c r="G29" s="94"/>
+      <c r="G29" s="81"/>
       <c r="DW29" s="33"/>
       <c r="DX29" s="33"/>
       <c r="DY29" s="33"/>
@@ -7819,25 +7843,25 @@
       <c r="EC29" s="33"/>
     </row>
     <row r="30" spans="1:133" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="94" t="s">
+      <c r="A30" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="81" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="94" t="s">
+      <c r="C30" s="81" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="98" t="s">
+      <c r="D30" s="85" t="s">
         <v>140</v>
       </c>
-      <c r="E30" s="94">
+      <c r="E30" s="81">
         <v>2</v>
       </c>
-      <c r="F30" s="94">
+      <c r="F30" s="81">
         <v>2</v>
       </c>
-      <c r="G30" s="94"/>
+      <c r="G30" s="81"/>
       <c r="DW30" s="33"/>
       <c r="DX30" s="33"/>
       <c r="DY30" s="33"/>
@@ -7894,10 +7918,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" s="11" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="93"/>
+      <c r="B2" s="103"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
     </row>

</xml_diff>